<commit_message>
QA Manage pages are working, but the page only updates after a 2nd change.
</commit_message>
<xml_diff>
--- a/composite/db_structure_quick.xlsx
+++ b/composite/db_structure_quick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Date Entered</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>q_owners</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
 </sst>
 </file>
@@ -419,25 +425,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -445,12 +452,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -458,33 +465,39 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -495,12 +508,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -511,12 +524,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -524,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>